<commit_message>
Prelim checkin -- before regenerating the csv files to pick up new default field values.
</commit_message>
<xml_diff>
--- a/app/tables/Tea_houses_editable/forms/Tea_houses_editable_form/Tea_houses_editable_form.xlsx
+++ b/app/tables/Tea_houses_editable/forms/Tea_houses_editable_form/Tea_houses_editable_form.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="32840" yWindow="2860" windowWidth="26640" windowHeight="20300" activeTab="1"/>
+    <workbookView xWindow="-10" yWindow="3670" windowWidth="16680" windowHeight="8260"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="3" r:id="rId2"/>
     <sheet name="settings" sheetId="4" r:id="rId3"/>
+    <sheet name="model" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
   <si>
     <t>type</t>
   </si>
@@ -113,15 +114,9 @@
     <t>Neighborhood</t>
   </si>
   <si>
-    <t>Latitude</t>
-  </si>
-  <si>
     <t>Latitude to edit</t>
   </si>
   <si>
-    <t>Longitude</t>
-  </si>
-  <si>
     <t>Longitude to edit</t>
   </si>
   <si>
@@ -198,13 +193,49 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>geopoint</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>model.isSessionVariable</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>data('Location.latitude')</t>
+  </si>
+  <si>
+    <t>data('Location.longitude')</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>TODO: enable saving with &lt;em&gt;assign Location_latitude data('lat')&lt;/em&gt; etc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -233,6 +264,12 @@
       <color theme="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -296,7 +333,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -313,6 +350,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -656,28 +694,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="41.83203125" customWidth="1"/>
-    <col min="7" max="7" width="40" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" customWidth="1"/>
+    <col min="5" max="6" width="18.1796875" customWidth="1"/>
+    <col min="7" max="7" width="41.81640625" customWidth="1"/>
+    <col min="8" max="8" width="40" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1">
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -688,27 +726,31 @@
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1">
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" ht="12">
+      <c r="F2" s="1"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
@@ -716,12 +758,13 @@
       <c r="E3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="73" customHeight="1">
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
@@ -729,34 +772,36 @@
       <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1">
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1">
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1">
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
@@ -764,12 +809,13 @@
       <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1">
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
@@ -777,12 +823,13 @@
       <c r="E8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4"/>
+      <c r="G8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1">
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
@@ -790,12 +837,13 @@
       <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4"/>
+      <c r="G9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1">
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
         <v>2</v>
       </c>
@@ -803,331 +851,408 @@
       <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4"/>
+      <c r="G10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1">
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
-        <v>21</v>
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>63</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1">
-      <c r="C13" s="4" t="s">
-        <v>48</v>
+      <c r="E12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" t="s">
+        <v>63</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="18" customHeight="1">
-      <c r="C14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="18" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="18" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="18" customHeight="1">
-      <c r="C17" s="4" t="s">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1">
-      <c r="C18" s="4" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1">
-      <c r="C19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1">
-      <c r="C20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1">
-      <c r="C21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="18" customHeight="1">
-      <c r="C22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" ht="18" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4" t="s">
+      <c r="F29" s="4"/>
+      <c r="G29" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" ht="18" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" ht="18" customHeight="1">
-      <c r="C25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" ht="18" customHeight="1">
-      <c r="C26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" ht="18" customHeight="1">
-      <c r="C27" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" ht="18" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" ht="18" customHeight="1">
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" ht="18" customHeight="1">
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" ht="18" customHeight="1">
-      <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" ht="18" customHeight="1">
+      <c r="F31" s="4"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="3:7" ht="18" customHeight="1">
+      <c r="F32" s="4"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="3:7" ht="18" customHeight="1">
+      <c r="F33" s="4"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="3:7" ht="18" customHeight="1">
+      <c r="F34" s="4"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="3:7" ht="18" customHeight="1">
+      <c r="F35" s="4"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="3:7" ht="18" customHeight="1">
+      <c r="F36" s="4"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="4"/>
-    </row>
-    <row r="38" spans="3:7" ht="18" customHeight="1">
+      <c r="F37" s="4"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="3:7" ht="36.75" customHeight="1">
+      <c r="F38" s="4"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="3:7" ht="18" customHeight="1">
+      <c r="F39" s="4"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="3:7" ht="18" customHeight="1"/>
-    <row r="42" spans="3:7" ht="18" customHeight="1"/>
-    <row r="43" spans="3:7" ht="62.5" customHeight="1"/>
-    <row r="44" spans="3:7" ht="42" customHeight="1"/>
-    <row r="45" spans="3:7" ht="40.75" customHeight="1">
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="3:7" ht="35.5" customHeight="1">
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="3:7" ht="34.25" customHeight="1">
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="3:7" ht="18" customHeight="1"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="3:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="3:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="3:8" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="3:8" ht="40.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="3:4" ht="35.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="3:4" ht="34.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1143,18 +1268,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="1" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.25" customHeight="1">
+    <row r="1" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1168,31 +1293,31 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="22.25" customHeight="1">
+    <row r="2" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="22.25" customHeight="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="22.25" customHeight="1"/>
-    <row r="5" spans="1:4" ht="22.25" customHeight="1"/>
-    <row r="6" spans="1:4" ht="22.25" customHeight="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1211,14 +1336,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -1229,7 +1354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1237,7 +1362,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1245,7 +1370,7 @@
         <v>20140204</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1254,17 +1379,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12.75" customHeight="1">
+    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A6" t="s">
-        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
@@ -1279,4 +1404,65 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="26.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>